<commit_message>
11.08.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Price list July 2020.xlsx
+++ b/2020/Others/Price list July 2020.xlsx
@@ -147,9 +147,6 @@
     <t>T180</t>
   </si>
   <si>
-    <t>July</t>
-  </si>
-  <si>
     <t>B68</t>
   </si>
   <si>
@@ -280,6 +277,9 @@
   </si>
   <si>
     <t>Lifting</t>
+  </si>
+  <si>
+    <t>August</t>
   </si>
 </sst>
 </file>
@@ -493,11 +493,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -511,11 +532,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -523,29 +544,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2904,8 +2904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2923,84 +2923,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
     </row>
     <row r="4" spans="1:15" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25">
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="30"/>
+      <c r="I4" s="14">
         <v>2020</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="21" customHeight="1">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="28" t="s">
+      <c r="D5" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="29" t="s">
-        <v>84</v>
+      <c r="I5" s="16" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="20.100000000000001" customHeight="1">
@@ -3039,7 +3039,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
       <c r="F7" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G7" s="7">
         <v>1040</v>
@@ -3085,7 +3085,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
       <c r="F9" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G9" s="7">
         <v>960</v>
@@ -3156,7 +3156,7 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G12" s="7">
         <v>5750</v>
@@ -3168,7 +3168,7 @@
     </row>
     <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="5">
         <v>760</v>
@@ -3179,7 +3179,7 @@
       <c r="D13" s="5"/>
       <c r="E13" s="6"/>
       <c r="F13" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G13" s="7">
         <v>1100</v>
@@ -3204,7 +3204,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
       <c r="F14" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G14" s="7">
         <v>1190</v>
@@ -3338,7 +3338,7 @@
     </row>
     <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="7">
         <v>970</v>
@@ -3349,7 +3349,7 @@
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
       <c r="F20" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G20" s="7">
         <v>4500</v>
@@ -3372,7 +3372,7 @@
       <c r="D21" s="5"/>
       <c r="E21" s="6"/>
       <c r="F21" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G21" s="7">
         <v>3620</v>
@@ -3395,7 +3395,7 @@
       <c r="D22" s="5"/>
       <c r="E22" s="6"/>
       <c r="F22" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G22" s="7">
         <v>4080</v>
@@ -3418,7 +3418,7 @@
       <c r="D23" s="5"/>
       <c r="E23" s="6"/>
       <c r="F23" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G23" s="7">
         <v>4220</v>
@@ -3441,7 +3441,7 @@
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
       <c r="F24" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G24" s="7">
         <v>3710</v>
@@ -3464,7 +3464,7 @@
       <c r="D25" s="5"/>
       <c r="E25" s="6"/>
       <c r="F25" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G25" s="7">
         <v>3640</v>
@@ -3476,7 +3476,7 @@
     </row>
     <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" s="5">
         <v>1170</v>
@@ -3487,7 +3487,7 @@
       <c r="D26" s="5"/>
       <c r="E26" s="6"/>
       <c r="F26" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G26" s="7">
         <v>3610</v>
@@ -3510,7 +3510,7 @@
       <c r="D27" s="5"/>
       <c r="E27" s="6"/>
       <c r="F27" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G27" s="7">
         <v>3890</v>
@@ -3533,7 +3533,7 @@
       <c r="D28" s="5"/>
       <c r="E28" s="6"/>
       <c r="F28" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G28" s="7">
         <v>4280</v>
@@ -3545,7 +3545,7 @@
     </row>
     <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" s="7">
         <v>2780</v>
@@ -3568,7 +3568,7 @@
     </row>
     <row r="30" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" s="7">
         <v>2770</v>
@@ -3581,7 +3581,7 @@
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G30" s="7">
         <v>4180</v>
@@ -3593,7 +3593,7 @@
     </row>
     <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31" s="7">
         <v>4050</v>
@@ -3604,7 +3604,7 @@
       <c r="D31" s="5"/>
       <c r="E31" s="6"/>
       <c r="F31" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G31" s="7">
         <v>5560</v>
@@ -3616,7 +3616,7 @@
     </row>
     <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" s="7">
         <v>6540</v>
@@ -3627,7 +3627,7 @@
       <c r="D32" s="5"/>
       <c r="E32" s="6"/>
       <c r="F32" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G32" s="7">
         <v>6090</v>
@@ -3639,7 +3639,7 @@
     </row>
     <row r="33" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B33" s="7">
         <v>5290</v>
@@ -3662,7 +3662,7 @@
     </row>
     <row r="34" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B34" s="7">
         <v>5010</v>
@@ -3673,7 +3673,7 @@
       <c r="D34" s="5"/>
       <c r="E34" s="6"/>
       <c r="F34" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G34" s="7">
         <v>7350</v>
@@ -3687,7 +3687,7 @@
     </row>
     <row r="35" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35" s="7">
         <v>5170</v>
@@ -3698,7 +3698,7 @@
       <c r="D35" s="5"/>
       <c r="E35" s="6"/>
       <c r="F35" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G35" s="7">
         <v>7890</v>
@@ -3710,7 +3710,7 @@
     </row>
     <row r="36" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B36" s="7">
         <v>7075</v>
@@ -3721,7 +3721,7 @@
       <c r="D36" s="5"/>
       <c r="E36" s="6"/>
       <c r="F36" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G36" s="7">
         <v>8310</v>
@@ -3733,7 +3733,7 @@
     </row>
     <row r="37" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B37" s="7">
         <v>5750</v>
@@ -3746,7 +3746,7 @@
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G37" s="7">
         <v>9300</v>
@@ -3758,7 +3758,7 @@
     </row>
     <row r="38" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B38" s="7">
         <v>4990</v>
@@ -3769,7 +3769,7 @@
       <c r="D38" s="5"/>
       <c r="E38" s="6"/>
       <c r="F38" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G38" s="7">
         <v>8310</v>
@@ -3781,7 +3781,7 @@
     </row>
     <row r="39" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B39" s="7">
         <v>5550</v>
@@ -3792,7 +3792,7 @@
       <c r="D39" s="5"/>
       <c r="E39" s="6"/>
       <c r="F39" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G39" s="7">
         <v>10340</v>
@@ -3804,7 +3804,7 @@
     </row>
     <row r="40" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B40" s="7">
         <v>5940</v>
@@ -3821,7 +3821,7 @@
     </row>
     <row r="41" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B41" s="7">
         <v>7890</v>
@@ -3838,7 +3838,7 @@
     </row>
     <row r="42" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B42" s="7">
         <v>9100</v>
@@ -3855,7 +3855,7 @@
     </row>
     <row r="43" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B43" s="7">
         <v>5510</v>
@@ -3872,7 +3872,7 @@
     </row>
     <row r="44" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B44" s="7">
         <v>6470</v>
@@ -3890,33 +3890,33 @@
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B45" s="19"/>
       <c r="C45" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D45" s="19"/>
       <c r="E45" s="19"/>
       <c r="F45" s="19"/>
       <c r="G45" s="19"/>
-      <c r="H45" s="15" t="s">
+      <c r="H45" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="I45" s="16"/>
+      <c r="I45" s="23"/>
       <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="27"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="18"/>
+      <c r="A46" s="20"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="25"/>
       <c r="J46" s="2"/>
     </row>
     <row r="47" spans="1:10">

</xml_diff>

<commit_message>
18.08.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Price list July 2020.xlsx
+++ b/2020/Others/Price list July 2020.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
   <si>
     <t>Model</t>
   </si>
@@ -280,6 +280,15 @@
   </si>
   <si>
     <t>August</t>
+  </si>
+  <si>
+    <t>L95</t>
+  </si>
+  <si>
+    <t>Z16_SKD</t>
+  </si>
+  <si>
+    <t>I12_SKD</t>
   </si>
 </sst>
 </file>
@@ -586,7 +595,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -607,7 +616,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -813,7 +822,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1914,7 +1923,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2354,7 +2363,7 @@
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2414,7 +2423,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2431,7 +2440,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2494,7 +2503,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2511,7 +2520,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2571,7 +2580,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2604,7 +2613,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2616,7 +2625,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2894,7 +2903,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2904,8 +2913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3016,15 +3025,17 @@
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
       <c r="F6" s="8" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="G6" s="7">
-        <v>1010</v>
+        <v>6470</v>
       </c>
       <c r="H6" s="7">
-        <v>1090</v>
-      </c>
-      <c r="I6" s="5"/>
+        <v>6990</v>
+      </c>
+      <c r="I6" s="5">
+        <v>400</v>
+      </c>
     </row>
     <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="8" t="s">
@@ -3039,13 +3050,13 @@
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
       <c r="F7" s="8" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="G7" s="7">
-        <v>1040</v>
+        <v>1070</v>
       </c>
       <c r="H7" s="7">
-        <v>1130</v>
+        <v>1160</v>
       </c>
       <c r="I7" s="5"/>
     </row>
@@ -3062,13 +3073,13 @@
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
       <c r="F8" s="8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G8" s="7">
-        <v>970</v>
+        <v>1160</v>
       </c>
       <c r="H8" s="7">
-        <v>1050</v>
+        <v>1250</v>
       </c>
       <c r="I8" s="5"/>
     </row>
@@ -3084,14 +3095,14 @@
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="9" t="s">
-        <v>60</v>
+      <c r="F9" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="G9" s="7">
-        <v>960</v>
+        <v>1010</v>
       </c>
       <c r="H9" s="7">
-        <v>1030</v>
+        <v>1090</v>
       </c>
       <c r="I9" s="5"/>
     </row>
@@ -3108,13 +3119,13 @@
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
       <c r="F10" s="8" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="G10" s="7">
-        <v>1070</v>
+        <v>1040</v>
       </c>
       <c r="H10" s="7">
-        <v>1160</v>
+        <v>1130</v>
       </c>
       <c r="I10" s="5"/>
     </row>
@@ -3130,14 +3141,14 @@
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="8" t="s">
-        <v>29</v>
+      <c r="F11" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="G11" s="7">
-        <v>1160</v>
+        <v>970</v>
       </c>
       <c r="H11" s="7">
-        <v>1250</v>
+        <v>1050</v>
       </c>
       <c r="I11" s="5"/>
     </row>
@@ -3156,13 +3167,13 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G12" s="7">
-        <v>5750</v>
+        <v>960</v>
       </c>
       <c r="H12" s="7">
-        <v>6190</v>
+        <v>1030</v>
       </c>
       <c r="I12" s="5"/>
     </row>
@@ -3179,49 +3190,43 @@
       <c r="D13" s="5"/>
       <c r="E13" s="6"/>
       <c r="F13" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13" s="7">
-        <v>1100</v>
-      </c>
-      <c r="H13" s="7">
-        <v>1190</v>
-      </c>
-      <c r="I13" s="5">
-        <v>45</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="5">
-        <v>920</v>
-      </c>
-      <c r="C14" s="5">
-        <v>990</v>
+        <v>41</v>
+      </c>
+      <c r="B14" s="7">
+        <v>970</v>
+      </c>
+      <c r="C14" s="7">
+        <v>1060</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
       <c r="F14" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G14" s="7">
-        <v>1190</v>
+        <v>5750</v>
       </c>
       <c r="H14" s="7">
-        <v>1290</v>
+        <v>6190</v>
       </c>
       <c r="I14" s="5">
-        <v>55</v>
+        <v>700</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B15" s="5">
-        <v>915</v>
+        <v>920</v>
       </c>
       <c r="C15" s="5">
         <v>990</v>
@@ -3229,133 +3234,137 @@
       <c r="D15" s="5"/>
       <c r="E15" s="6"/>
       <c r="F15" s="8" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="G15" s="7">
-        <v>1250</v>
+        <v>1190</v>
       </c>
       <c r="H15" s="7">
-        <v>1350</v>
-      </c>
-      <c r="I15" s="5"/>
+        <v>1290</v>
+      </c>
+      <c r="I15" s="5">
+        <v>55</v>
+      </c>
       <c r="O15" s="11" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" s="5">
-        <v>920</v>
+        <v>915</v>
       </c>
       <c r="C16" s="5">
-        <v>999</v>
+        <v>990</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
       <c r="F16" s="8" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="G16" s="7">
-        <v>1370</v>
+        <v>1100</v>
       </c>
       <c r="H16" s="7">
-        <v>1490</v>
-      </c>
-      <c r="I16" s="5"/>
+        <v>1190</v>
+      </c>
+      <c r="I16" s="5">
+        <v>45</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="8" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B17" s="5">
-        <v>880</v>
+        <v>920</v>
       </c>
       <c r="C17" s="5">
-        <v>950</v>
+        <v>999</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="6"/>
       <c r="F17" s="8" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="G17" s="7">
-        <v>1220</v>
+        <v>1250</v>
       </c>
       <c r="H17" s="7">
-        <v>1320</v>
+        <v>1350</v>
       </c>
       <c r="I17" s="5"/>
     </row>
     <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B18" s="5">
-        <v>845</v>
+        <v>880</v>
       </c>
       <c r="C18" s="5">
-        <v>910</v>
-      </c>
-      <c r="D18" s="5">
-        <v>25</v>
-      </c>
+        <v>950</v>
+      </c>
+      <c r="D18" s="5"/>
       <c r="E18" s="6"/>
       <c r="F18" s="8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G18" s="7">
-        <v>3560</v>
+        <v>1370</v>
       </c>
       <c r="H18" s="7">
-        <v>3840</v>
+        <v>1490</v>
       </c>
       <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B19" s="5">
-        <v>820</v>
+        <v>845</v>
       </c>
       <c r="C19" s="5">
-        <v>890</v>
-      </c>
-      <c r="D19" s="5"/>
+        <v>910</v>
+      </c>
+      <c r="D19" s="5">
+        <v>25</v>
+      </c>
       <c r="E19" s="6"/>
       <c r="F19" s="8" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="G19" s="7">
-        <v>3340</v>
+        <v>1220</v>
       </c>
       <c r="H19" s="7">
-        <v>3590</v>
+        <v>1320</v>
       </c>
       <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="7">
-        <v>970</v>
-      </c>
-      <c r="C20" s="7">
-        <v>1060</v>
+        <v>32</v>
+      </c>
+      <c r="B20" s="5">
+        <v>820</v>
+      </c>
+      <c r="C20" s="5">
+        <v>890</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
       <c r="F20" s="8" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="G20" s="7">
-        <v>4500</v>
+        <v>3610</v>
       </c>
       <c r="H20" s="7">
-        <v>4790</v>
+        <v>3890</v>
       </c>
       <c r="I20" s="5"/>
     </row>
@@ -3371,14 +3380,14 @@
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="8" t="s">
-        <v>65</v>
+      <c r="F21" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="G21" s="7">
-        <v>3620</v>
+        <v>3890</v>
       </c>
       <c r="H21" s="7">
-        <v>3890</v>
+        <v>4190</v>
       </c>
       <c r="I21" s="5"/>
     </row>
@@ -3395,13 +3404,13 @@
       <c r="D22" s="5"/>
       <c r="E22" s="6"/>
       <c r="F22" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G22" s="7">
-        <v>4080</v>
+        <v>4280</v>
       </c>
       <c r="H22" s="7">
-        <v>4390</v>
+        <v>4590</v>
       </c>
       <c r="I22" s="5"/>
     </row>
@@ -3418,13 +3427,13 @@
       <c r="D23" s="5"/>
       <c r="E23" s="6"/>
       <c r="F23" s="8" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="G23" s="7">
-        <v>4220</v>
+        <v>5020</v>
       </c>
       <c r="H23" s="7">
-        <v>4540</v>
+        <v>5390</v>
       </c>
       <c r="I23" s="5"/>
     </row>
@@ -3441,13 +3450,13 @@
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
       <c r="F24" s="8" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="G24" s="7">
-        <v>3710</v>
+        <v>4180</v>
       </c>
       <c r="H24" s="7">
-        <v>3990</v>
+        <v>4490</v>
       </c>
       <c r="I24" s="5"/>
     </row>
@@ -3464,13 +3473,13 @@
       <c r="D25" s="5"/>
       <c r="E25" s="6"/>
       <c r="F25" s="8" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="G25" s="7">
-        <v>3640</v>
+        <v>5560</v>
       </c>
       <c r="H25" s="7">
-        <v>3890</v>
+        <v>5990</v>
       </c>
       <c r="I25" s="5"/>
     </row>
@@ -3487,13 +3496,13 @@
       <c r="D26" s="5"/>
       <c r="E26" s="6"/>
       <c r="F26" s="8" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="G26" s="7">
-        <v>3610</v>
+        <v>6090</v>
       </c>
       <c r="H26" s="7">
-        <v>3890</v>
+        <v>6590</v>
       </c>
       <c r="I26" s="5"/>
     </row>
@@ -3510,13 +3519,13 @@
       <c r="D27" s="5"/>
       <c r="E27" s="6"/>
       <c r="F27" s="8" t="s">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="G27" s="7">
-        <v>3890</v>
+        <v>5390</v>
       </c>
       <c r="H27" s="7">
-        <v>4190</v>
+        <v>5790</v>
       </c>
       <c r="I27" s="5"/>
     </row>
@@ -3533,13 +3542,13 @@
       <c r="D28" s="5"/>
       <c r="E28" s="6"/>
       <c r="F28" s="8" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="G28" s="7">
-        <v>4280</v>
+        <v>3560</v>
       </c>
       <c r="H28" s="7">
-        <v>4590</v>
+        <v>3840</v>
       </c>
       <c r="I28" s="5"/>
     </row>
@@ -3553,16 +3562,18 @@
       <c r="C29" s="7">
         <v>2990</v>
       </c>
-      <c r="D29" s="5"/>
+      <c r="D29" s="5">
+        <v>450</v>
+      </c>
       <c r="E29" s="6"/>
-      <c r="F29" s="10" t="s">
-        <v>9</v>
+      <c r="F29" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="G29" s="7">
-        <v>5020</v>
+        <v>3340</v>
       </c>
       <c r="H29" s="7">
-        <v>5390</v>
+        <v>3590</v>
       </c>
       <c r="I29" s="5"/>
     </row>
@@ -3581,13 +3592,13 @@
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="8" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G30" s="7">
-        <v>4180</v>
+        <v>4500</v>
       </c>
       <c r="H30" s="7">
-        <v>4490</v>
+        <v>4790</v>
       </c>
       <c r="I30" s="5"/>
     </row>
@@ -3604,13 +3615,13 @@
       <c r="D31" s="5"/>
       <c r="E31" s="6"/>
       <c r="F31" s="8" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G31" s="7">
-        <v>5560</v>
+        <v>3620</v>
       </c>
       <c r="H31" s="7">
-        <v>5990</v>
+        <v>3890</v>
       </c>
       <c r="I31" s="5"/>
     </row>
@@ -3627,241 +3638,259 @@
       <c r="D32" s="5"/>
       <c r="E32" s="6"/>
       <c r="F32" s="8" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G32" s="7">
-        <v>6090</v>
+        <v>4080</v>
       </c>
       <c r="H32" s="7">
-        <v>6590</v>
+        <v>4390</v>
       </c>
       <c r="I32" s="5"/>
     </row>
     <row r="33" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="8" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="B33" s="7">
-        <v>5290</v>
+        <v>4150</v>
       </c>
       <c r="C33" s="7">
-        <v>5690</v>
+        <v>4390</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="6"/>
       <c r="F33" s="8" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="G33" s="7">
-        <v>5390</v>
+        <v>4220</v>
       </c>
       <c r="H33" s="7">
-        <v>5790</v>
+        <v>4540</v>
       </c>
       <c r="I33" s="5"/>
     </row>
     <row r="34" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="7">
-        <v>5010</v>
+        <v>5290</v>
       </c>
       <c r="C34" s="7">
-        <v>5390</v>
+        <v>5690</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="6"/>
       <c r="F34" s="8" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="G34" s="7">
-        <v>7350</v>
+        <v>3640</v>
       </c>
       <c r="H34" s="7">
-        <v>7990</v>
-      </c>
-      <c r="I34" s="5">
-        <v>700</v>
-      </c>
+        <v>3890</v>
+      </c>
+      <c r="I34" s="5"/>
     </row>
     <row r="35" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" s="7">
-        <v>5170</v>
+        <v>5010</v>
       </c>
       <c r="C35" s="7">
-        <v>5499</v>
+        <v>5390</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="6"/>
       <c r="F35" s="8" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="G35" s="7">
-        <v>7890</v>
+        <v>3710</v>
       </c>
       <c r="H35" s="7">
-        <v>8490</v>
+        <v>3990</v>
       </c>
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="7">
-        <v>7075</v>
+        <v>5170</v>
       </c>
       <c r="C36" s="7">
-        <v>7575</v>
+        <v>5499</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="6"/>
       <c r="F36" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G36" s="7">
-        <v>8310</v>
+        <v>7350</v>
       </c>
       <c r="H36" s="7">
-        <v>8990</v>
-      </c>
-      <c r="I36" s="5"/>
+        <v>7990</v>
+      </c>
+      <c r="I36" s="5">
+        <v>700</v>
+      </c>
     </row>
     <row r="37" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="7">
-        <v>5750</v>
+        <v>7075</v>
       </c>
       <c r="C37" s="7">
-        <v>6190</v>
-      </c>
-      <c r="D37" s="5">
-        <v>550</v>
-      </c>
+        <v>7575</v>
+      </c>
+      <c r="D37" s="5"/>
       <c r="E37" s="6"/>
       <c r="F37" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G37" s="7">
-        <v>9300</v>
+        <v>7890</v>
       </c>
       <c r="H37" s="7">
-        <v>9790</v>
+        <v>8490</v>
       </c>
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" s="7">
-        <v>4990</v>
+        <v>5750</v>
       </c>
       <c r="C38" s="7">
-        <v>5290</v>
-      </c>
-      <c r="D38" s="5"/>
+        <v>6190</v>
+      </c>
+      <c r="D38" s="5">
+        <v>550</v>
+      </c>
       <c r="E38" s="6"/>
       <c r="F38" s="8" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="G38" s="7">
-        <v>8310</v>
+        <v>7790</v>
       </c>
       <c r="H38" s="7">
-        <v>8990</v>
+        <v>8290</v>
       </c>
       <c r="I38" s="5"/>
     </row>
     <row r="39" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" s="7">
-        <v>5550</v>
+        <v>4990</v>
       </c>
       <c r="C39" s="7">
-        <v>5990</v>
+        <v>5290</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="6"/>
       <c r="F39" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G39" s="7">
-        <v>10340</v>
+        <v>8310</v>
       </c>
       <c r="H39" s="7">
-        <v>10990</v>
+        <v>8990</v>
       </c>
       <c r="I39" s="5"/>
     </row>
     <row r="40" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" s="7">
-        <v>5940</v>
+        <v>5550</v>
       </c>
       <c r="C40" s="7">
-        <v>6390</v>
+        <v>5990</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="6"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
+      <c r="F40" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G40" s="7">
+        <v>8310</v>
+      </c>
+      <c r="H40" s="7">
+        <v>8990</v>
+      </c>
       <c r="I40" s="5"/>
     </row>
     <row r="41" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B41" s="7">
-        <v>7890</v>
+        <v>5940</v>
       </c>
       <c r="C41" s="7">
-        <v>8490</v>
+        <v>6390</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="6"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
+      <c r="F41" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G41" s="7">
+        <v>9300</v>
+      </c>
+      <c r="H41" s="7">
+        <v>9790</v>
+      </c>
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B42" s="7">
-        <v>9100</v>
+        <v>7890</v>
       </c>
       <c r="C42" s="7">
-        <v>9790</v>
+        <v>8490</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="6"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
+      <c r="F42" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G42" s="7">
+        <v>10340</v>
+      </c>
+      <c r="H42" s="7">
+        <v>10990</v>
+      </c>
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B43" s="7">
-        <v>5510</v>
+        <v>9100</v>
       </c>
       <c r="C43" s="7">
-        <v>5890</v>
+        <v>9790</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="6"/>
@@ -3872,17 +3901,15 @@
     </row>
     <row r="44" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B44" s="7">
-        <v>6470</v>
+        <v>5510</v>
       </c>
       <c r="C44" s="7">
-        <v>6990</v>
-      </c>
-      <c r="D44" s="5">
-        <v>400</v>
-      </c>
+        <v>5890</v>
+      </c>
+      <c r="D44" s="5"/>
       <c r="E44" s="6"/>
       <c r="F44" s="8"/>
       <c r="G44" s="7"/>
@@ -3923,6 +3950,9 @@
       <c r="J47" s="1"/>
     </row>
   </sheetData>
+  <sortState ref="A6:D44">
+    <sortCondition ref="A6"/>
+  </sortState>
   <mergeCells count="8">
     <mergeCell ref="A45:B46"/>
     <mergeCell ref="C45:G46"/>

</xml_diff>

<commit_message>
24.08.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Price list July 2020.xlsx
+++ b/2020/Others/Price list July 2020.xlsx
@@ -595,7 +595,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -616,7 +616,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -822,7 +822,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1923,7 +1923,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2363,7 +2363,7 @@
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2423,7 +2423,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2440,7 +2440,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2503,7 +2503,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2520,7 +2520,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2580,7 +2580,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2613,7 +2613,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2625,7 +2625,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2903,7 +2903,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2914,7 +2914,7 @@
   <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I46"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3192,8 +3192,12 @@
       <c r="F13" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="G13" s="7">
+        <v>1080</v>
+      </c>
+      <c r="H13" s="7">
+        <v>1150</v>
+      </c>
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:15" ht="20.100000000000001" customHeight="1">

</xml_diff>

<commit_message>
29.08.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Price list July 2020.xlsx
+++ b/2020/Others/Price list July 2020.xlsx
@@ -279,9 +279,6 @@
     <t>Lifting</t>
   </si>
   <si>
-    <t>August</t>
-  </si>
-  <si>
     <t>L95</t>
   </si>
   <si>
@@ -289,15 +286,17 @@
   </si>
   <si>
     <t>I12_SKD</t>
+  </si>
+  <si>
+    <t>i99</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -383,7 +382,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -468,13 +467,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -504,9 +540,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -553,8 +586,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -595,7 +634,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -616,7 +655,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -822,7 +861,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1923,7 +1962,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2363,7 +2402,7 @@
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2423,7 +2462,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2440,7 +2479,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2503,7 +2542,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2520,7 +2559,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2580,7 +2619,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2613,7 +2652,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2625,7 +2664,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2903,7 +2942,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2913,8 +2952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2932,83 +2971,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:15" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
-      <c r="G4" s="30" t="s">
-        <v>84</v>
+      <c r="G4" s="29">
+        <v>2020</v>
       </c>
       <c r="H4" s="30"/>
-      <c r="I4" s="14">
-        <v>2020</v>
-      </c>
+      <c r="I4" s="31"/>
     </row>
     <row r="5" spans="1:15" ht="21" customHeight="1">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="15" t="s">
+      <c r="E5" s="16"/>
+      <c r="F5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="15" t="s">
         <v>83</v>
       </c>
     </row>
@@ -3050,14 +3087,10 @@
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
       <c r="F7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="7">
-        <v>1070</v>
-      </c>
-      <c r="H7" s="7">
-        <v>1160</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:15" ht="20.100000000000001" customHeight="1">
@@ -3073,13 +3106,13 @@
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
       <c r="F8" s="8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="G8" s="7">
+        <v>1070</v>
+      </c>
+      <c r="H8" s="7">
         <v>1160</v>
-      </c>
-      <c r="H8" s="7">
-        <v>1250</v>
       </c>
       <c r="I8" s="5"/>
     </row>
@@ -3096,13 +3129,13 @@
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
       <c r="F9" s="8" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="G9" s="7">
-        <v>1010</v>
+        <v>1160</v>
       </c>
       <c r="H9" s="7">
-        <v>1090</v>
+        <v>1250</v>
       </c>
       <c r="I9" s="5"/>
     </row>
@@ -3119,13 +3152,13 @@
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
       <c r="F10" s="8" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="G10" s="7">
-        <v>1040</v>
+        <v>1010</v>
       </c>
       <c r="H10" s="7">
-        <v>1130</v>
+        <v>1090</v>
       </c>
       <c r="I10" s="5"/>
     </row>
@@ -3142,13 +3175,13 @@
       <c r="D11" s="5"/>
       <c r="E11" s="6"/>
       <c r="F11" s="9" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="G11" s="7">
-        <v>970</v>
+        <v>1040</v>
       </c>
       <c r="H11" s="7">
-        <v>1050</v>
+        <v>1130</v>
       </c>
       <c r="I11" s="5"/>
     </row>
@@ -3167,13 +3200,13 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="8" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="G12" s="7">
-        <v>960</v>
+        <v>970</v>
       </c>
       <c r="H12" s="7">
-        <v>1030</v>
+        <v>1050</v>
       </c>
       <c r="I12" s="5"/>
     </row>
@@ -3190,13 +3223,13 @@
       <c r="D13" s="5"/>
       <c r="E13" s="6"/>
       <c r="F13" s="8" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="G13" s="7">
-        <v>1080</v>
+        <v>960</v>
       </c>
       <c r="H13" s="7">
-        <v>1150</v>
+        <v>1030</v>
       </c>
       <c r="I13" s="5"/>
     </row>
@@ -3213,17 +3246,15 @@
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
       <c r="F14" s="8" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="G14" s="7">
-        <v>5750</v>
+        <v>1080</v>
       </c>
       <c r="H14" s="7">
-        <v>6190</v>
-      </c>
-      <c r="I14" s="5">
-        <v>700</v>
-      </c>
+        <v>1150</v>
+      </c>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="8" t="s">
@@ -3238,16 +3269,16 @@
       <c r="D15" s="5"/>
       <c r="E15" s="6"/>
       <c r="F15" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G15" s="7">
-        <v>1190</v>
+        <v>5750</v>
       </c>
       <c r="H15" s="7">
-        <v>1290</v>
+        <v>6190</v>
       </c>
       <c r="I15" s="5">
-        <v>55</v>
+        <v>700</v>
       </c>
       <c r="O15" s="11" t="s">
         <v>36</v>
@@ -3266,16 +3297,16 @@
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
       <c r="F16" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G16" s="7">
-        <v>1100</v>
+        <v>1190</v>
       </c>
       <c r="H16" s="7">
-        <v>1190</v>
+        <v>1290</v>
       </c>
       <c r="I16" s="5">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1">
@@ -3291,15 +3322,17 @@
       <c r="D17" s="5"/>
       <c r="E17" s="6"/>
       <c r="F17" s="8" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="G17" s="7">
-        <v>1250</v>
+        <v>1100</v>
       </c>
       <c r="H17" s="7">
-        <v>1350</v>
-      </c>
-      <c r="I17" s="5"/>
+        <v>1190</v>
+      </c>
+      <c r="I17" s="5">
+        <v>45</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="8" t="s">
@@ -3314,13 +3347,13 @@
       <c r="D18" s="5"/>
       <c r="E18" s="6"/>
       <c r="F18" s="8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G18" s="7">
-        <v>1370</v>
+        <v>1250</v>
       </c>
       <c r="H18" s="7">
-        <v>1490</v>
+        <v>1350</v>
       </c>
       <c r="I18" s="5"/>
     </row>
@@ -3339,13 +3372,13 @@
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="8" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="G19" s="7">
-        <v>1220</v>
+        <v>1370</v>
       </c>
       <c r="H19" s="7">
-        <v>1320</v>
+        <v>1490</v>
       </c>
       <c r="I19" s="5"/>
     </row>
@@ -3362,13 +3395,13 @@
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
       <c r="F20" s="8" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="G20" s="7">
-        <v>3610</v>
+        <v>1220</v>
       </c>
       <c r="H20" s="7">
-        <v>3890</v>
+        <v>1320</v>
       </c>
       <c r="I20" s="5"/>
     </row>
@@ -3385,13 +3418,13 @@
       <c r="D21" s="5"/>
       <c r="E21" s="6"/>
       <c r="F21" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G21" s="7">
+        <v>3610</v>
+      </c>
+      <c r="H21" s="7">
         <v>3890</v>
-      </c>
-      <c r="H21" s="7">
-        <v>4190</v>
       </c>
       <c r="I21" s="5"/>
     </row>
@@ -3408,13 +3441,13 @@
       <c r="D22" s="5"/>
       <c r="E22" s="6"/>
       <c r="F22" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G22" s="7">
-        <v>4280</v>
+        <v>3890</v>
       </c>
       <c r="H22" s="7">
-        <v>4590</v>
+        <v>4190</v>
       </c>
       <c r="I22" s="5"/>
     </row>
@@ -3431,13 +3464,13 @@
       <c r="D23" s="5"/>
       <c r="E23" s="6"/>
       <c r="F23" s="8" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="G23" s="7">
-        <v>5020</v>
+        <v>4280</v>
       </c>
       <c r="H23" s="7">
-        <v>5390</v>
+        <v>4590</v>
       </c>
       <c r="I23" s="5"/>
     </row>
@@ -3454,13 +3487,13 @@
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
       <c r="F24" s="8" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="G24" s="7">
-        <v>4180</v>
+        <v>5020</v>
       </c>
       <c r="H24" s="7">
-        <v>4490</v>
+        <v>5390</v>
       </c>
       <c r="I24" s="5"/>
     </row>
@@ -3477,13 +3510,13 @@
       <c r="D25" s="5"/>
       <c r="E25" s="6"/>
       <c r="F25" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G25" s="7">
-        <v>5560</v>
+        <v>4180</v>
       </c>
       <c r="H25" s="7">
-        <v>5990</v>
+        <v>4490</v>
       </c>
       <c r="I25" s="5"/>
     </row>
@@ -3500,13 +3533,13 @@
       <c r="D26" s="5"/>
       <c r="E26" s="6"/>
       <c r="F26" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G26" s="7">
-        <v>6090</v>
+        <v>5560</v>
       </c>
       <c r="H26" s="7">
-        <v>6590</v>
+        <v>5990</v>
       </c>
       <c r="I26" s="5"/>
     </row>
@@ -3523,13 +3556,13 @@
       <c r="D27" s="5"/>
       <c r="E27" s="6"/>
       <c r="F27" s="8" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="G27" s="7">
-        <v>5390</v>
+        <v>6090</v>
       </c>
       <c r="H27" s="7">
-        <v>5790</v>
+        <v>6590</v>
       </c>
       <c r="I27" s="5"/>
     </row>
@@ -3546,13 +3579,13 @@
       <c r="D28" s="5"/>
       <c r="E28" s="6"/>
       <c r="F28" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G28" s="7">
-        <v>3560</v>
+        <v>5390</v>
       </c>
       <c r="H28" s="7">
-        <v>3840</v>
+        <v>5790</v>
       </c>
       <c r="I28" s="5"/>
     </row>
@@ -3571,13 +3604,13 @@
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="8" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G29" s="7">
-        <v>3340</v>
+        <v>3560</v>
       </c>
       <c r="H29" s="7">
-        <v>3590</v>
+        <v>3840</v>
       </c>
       <c r="I29" s="5"/>
     </row>
@@ -3596,13 +3629,13 @@
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="8" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="G30" s="7">
-        <v>4500</v>
+        <v>3340</v>
       </c>
       <c r="H30" s="7">
-        <v>4790</v>
+        <v>3590</v>
       </c>
       <c r="I30" s="5"/>
     </row>
@@ -3619,13 +3652,13 @@
       <c r="D31" s="5"/>
       <c r="E31" s="6"/>
       <c r="F31" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G31" s="7">
-        <v>3620</v>
+        <v>4500</v>
       </c>
       <c r="H31" s="7">
-        <v>3890</v>
+        <v>4790</v>
       </c>
       <c r="I31" s="5"/>
     </row>
@@ -3642,19 +3675,19 @@
       <c r="D32" s="5"/>
       <c r="E32" s="6"/>
       <c r="F32" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G32" s="7">
-        <v>4080</v>
+        <v>3620</v>
       </c>
       <c r="H32" s="7">
-        <v>4390</v>
+        <v>3890</v>
       </c>
       <c r="I32" s="5"/>
     </row>
     <row r="33" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B33" s="7">
         <v>4150</v>
@@ -3665,13 +3698,13 @@
       <c r="D33" s="5"/>
       <c r="E33" s="6"/>
       <c r="F33" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G33" s="7">
-        <v>4220</v>
+        <v>4080</v>
       </c>
       <c r="H33" s="7">
-        <v>4540</v>
+        <v>4390</v>
       </c>
       <c r="I33" s="5"/>
     </row>
@@ -3688,13 +3721,13 @@
       <c r="D34" s="5"/>
       <c r="E34" s="6"/>
       <c r="F34" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G34" s="7">
-        <v>3640</v>
+        <v>4220</v>
       </c>
       <c r="H34" s="7">
-        <v>3890</v>
+        <v>4540</v>
       </c>
       <c r="I34" s="5"/>
     </row>
@@ -3711,13 +3744,13 @@
       <c r="D35" s="5"/>
       <c r="E35" s="6"/>
       <c r="F35" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G35" s="7">
-        <v>3710</v>
+        <v>3640</v>
       </c>
       <c r="H35" s="7">
-        <v>3990</v>
+        <v>3890</v>
       </c>
       <c r="I35" s="5"/>
     </row>
@@ -3734,17 +3767,15 @@
       <c r="D36" s="5"/>
       <c r="E36" s="6"/>
       <c r="F36" s="8" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G36" s="7">
-        <v>7350</v>
+        <v>3710</v>
       </c>
       <c r="H36" s="7">
-        <v>7990</v>
-      </c>
-      <c r="I36" s="5">
-        <v>700</v>
-      </c>
+        <v>3990</v>
+      </c>
+      <c r="I36" s="5"/>
     </row>
     <row r="37" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="8" t="s">
@@ -3759,15 +3790,17 @@
       <c r="D37" s="5"/>
       <c r="E37" s="6"/>
       <c r="F37" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G37" s="7">
-        <v>7890</v>
+        <v>7350</v>
       </c>
       <c r="H37" s="7">
-        <v>8490</v>
-      </c>
-      <c r="I37" s="5"/>
+        <v>7990</v>
+      </c>
+      <c r="I37" s="5">
+        <v>700</v>
+      </c>
     </row>
     <row r="38" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="8" t="s">
@@ -3784,13 +3817,13 @@
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="8" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G38" s="7">
-        <v>7790</v>
+        <v>7890</v>
       </c>
       <c r="H38" s="7">
-        <v>8290</v>
+        <v>8490</v>
       </c>
       <c r="I38" s="5"/>
     </row>
@@ -3807,13 +3840,13 @@
       <c r="D39" s="5"/>
       <c r="E39" s="6"/>
       <c r="F39" s="8" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="G39" s="7">
-        <v>8310</v>
+        <v>7790</v>
       </c>
       <c r="H39" s="7">
-        <v>8990</v>
+        <v>8290</v>
       </c>
       <c r="I39" s="5"/>
     </row>
@@ -3830,7 +3863,7 @@
       <c r="D40" s="5"/>
       <c r="E40" s="6"/>
       <c r="F40" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G40" s="7">
         <v>8310</v>
@@ -3853,13 +3886,13 @@
       <c r="D41" s="5"/>
       <c r="E41" s="6"/>
       <c r="F41" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G41" s="7">
-        <v>9300</v>
+        <v>8310</v>
       </c>
       <c r="H41" s="7">
-        <v>9790</v>
+        <v>8990</v>
       </c>
       <c r="I41" s="5"/>
     </row>
@@ -3876,13 +3909,13 @@
       <c r="D42" s="5"/>
       <c r="E42" s="6"/>
       <c r="F42" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G42" s="7">
-        <v>10340</v>
+        <v>9300</v>
       </c>
       <c r="H42" s="7">
-        <v>10990</v>
+        <v>9790</v>
       </c>
       <c r="I42" s="5"/>
     </row>
@@ -3898,9 +3931,15 @@
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="6"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
+      <c r="F43" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G43" s="7">
+        <v>10340</v>
+      </c>
+      <c r="H43" s="7">
+        <v>10990</v>
+      </c>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="1:10" ht="20.100000000000001" customHeight="1">
@@ -3921,33 +3960,33 @@
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19" t="s">
+      <c r="B45" s="18"/>
+      <c r="C45" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="22" t="s">
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I45" s="23"/>
+      <c r="I45" s="22"/>
       <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="20"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="25"/>
+      <c r="A46" s="19"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="24"/>
       <c r="J46" s="2"/>
     </row>
     <row r="47" spans="1:10">
@@ -3965,7 +4004,7 @@
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A4:D4"/>
-    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G4:I4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>